<commit_message>
Se actualizo el excel de caracteristicas de renta
</commit_message>
<xml_diff>
--- a/scrapers/Características_Renta.xlsx
+++ b/scrapers/Características_Renta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\futbo\Documents\Focoasset archivos\scrapers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\futbo\Documents\Focoasset archivos\work\scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10E2E939-C5BF-4C6E-A629-54E978E9A909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C30768-8B22-4030-9FB2-72EEC58EE030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Mínimo</t>
   </si>
@@ -78,9 +78,6 @@
     <t>tipo_transaccion</t>
   </si>
   <si>
-    <t>estado_uso</t>
-  </si>
-  <si>
     <t>bono_pie_inmo</t>
   </si>
   <si>
@@ -115,6 +112,15 @@
   </si>
   <si>
     <t>Si esta en todas las propiedades</t>
+  </si>
+  <si>
+    <t>estado_uso*</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>No especifica si es nuevo pero si tiene el año de construccion</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -182,13 +194,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +485,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,99 +512,105 @@
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="F7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -601,13 +620,13 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
+      <c r="A15" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
+      <c r="A16" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>